<commit_message>
Updates to indexing demo.
</commit_message>
<xml_diff>
--- a/Articles/Brockway_Landscape_2017/data/IndexingDemoRawData.xlsx
+++ b/Articles/Brockway_Landscape_2017/data/IndexingDemoRawData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/Documents/Calvin stuff/Conferences and Papers/2016 CES Landscape Paper/Response to reviewer about indexing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/Econ-Growth-R-Analysis/Articles/Brockway_Landscape_2017/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -126,12 +126,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>MKH:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+IEA total primary energy supply in PJ.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="12">
   <si>
     <t>Year</t>
   </si>
@@ -161,6 +183,12 @@
   </si>
   <si>
     <t>K</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>iE</t>
   </si>
 </sst>
 </file>
@@ -233,13 +261,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -522,22 +556,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="8.83203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.83203125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="2"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -556,17 +591,23 @@
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1960</v>
       </c>
@@ -586,25 +627,32 @@
       <c r="F2" s="1">
         <v>53787719349.746696</v>
       </c>
-      <c r="G2" s="2">
-        <f>D2/D$2</f>
+      <c r="G2" s="5">
+        <v>6653.5788240000002</v>
+      </c>
+      <c r="H2" s="2">
+        <f t="shared" ref="H2:H33" si="0">D2/D$2</f>
         <v>1</v>
       </c>
-      <c r="H2" s="2">
-        <f>E2/E$2</f>
+      <c r="I2" s="2">
+        <f t="shared" ref="I2:I33" si="1">E2/E$2</f>
         <v>1</v>
       </c>
-      <c r="I2" s="2">
-        <f>F2/F$2</f>
+      <c r="J2" s="2">
+        <f t="shared" ref="J2:K33" si="2">F2/F$2</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K2" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1961</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" ref="B3:B53" si="0">A3-A$2</f>
+        <f t="shared" ref="B3:B52" si="3">A3-A$2</f>
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -619,25 +667,32 @@
       <c r="F3" s="1">
         <v>53532935329.551628</v>
       </c>
-      <c r="G3" s="2">
-        <f>D3/D$2</f>
+      <c r="G3" s="5">
+        <v>6646.6706040000008</v>
+      </c>
+      <c r="H3" s="2">
+        <f t="shared" si="0"/>
         <v>1.0215423519722242</v>
       </c>
-      <c r="H3" s="2">
-        <f>E3/E$2</f>
+      <c r="I3" s="2">
+        <f t="shared" si="1"/>
         <v>1.0406303578995608</v>
       </c>
-      <c r="I3" s="2">
-        <f>F3/F$2</f>
+      <c r="J3" s="2">
+        <f t="shared" si="2"/>
         <v>0.99526315628780659</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K3" s="2">
+        <f t="shared" si="2"/>
+        <v>0.998961728690268</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1962</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -652,25 +707,32 @@
       <c r="F4" s="1">
         <v>53484488949.737625</v>
       </c>
-      <c r="G4" s="2">
-        <f>D4/D$2</f>
+      <c r="G4" s="5">
+        <v>6883.2248040000004</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" si="0"/>
         <v>1.0395224686652205</v>
       </c>
-      <c r="H4" s="2">
-        <f>E4/E$2</f>
+      <c r="I4" s="2">
+        <f t="shared" si="1"/>
         <v>1.0683501759304703</v>
       </c>
-      <c r="I4" s="2">
-        <f>F4/F$2</f>
+      <c r="J4" s="2">
+        <f t="shared" si="2"/>
         <v>0.9943624603594482</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K4" s="2">
+        <f t="shared" si="2"/>
+        <v>1.0345146553568507</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1963</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -685,25 +747,32 @@
       <c r="F5" s="1">
         <v>53801946633.701302</v>
       </c>
-      <c r="G5" s="2">
-        <f>D5/D$2</f>
+      <c r="G5" s="5">
+        <v>7180.7806800000008</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="0"/>
         <v>1.0797278937580403</v>
       </c>
-      <c r="H5" s="2">
-        <f>E5/E$2</f>
+      <c r="I5" s="2">
+        <f t="shared" si="1"/>
         <v>1.1022647076922616</v>
       </c>
-      <c r="I5" s="2">
-        <f>F5/F$2</f>
+      <c r="J5" s="2">
+        <f t="shared" si="2"/>
         <v>1.0002645080350423</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K5" s="2">
+        <f t="shared" si="2"/>
+        <v>1.0792358323160374</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1964</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -718,25 +787,32 @@
       <c r="F6" s="1">
         <v>54485444316.787704</v>
       </c>
-      <c r="G6" s="2">
-        <f>D6/D$2</f>
+      <c r="G6" s="5">
+        <v>7263.1350360000006</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="0"/>
         <v>1.1403442439458449</v>
       </c>
-      <c r="H6" s="2">
-        <f>E6/E$2</f>
+      <c r="I6" s="2">
+        <f t="shared" si="1"/>
         <v>1.1537099491144942</v>
       </c>
-      <c r="I6" s="2">
-        <f>F6/F$2</f>
+      <c r="J6" s="2">
+        <f t="shared" si="2"/>
         <v>1.0129718265707486</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K6" s="2">
+        <f t="shared" si="2"/>
+        <v>1.0916132848387219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1965</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -751,25 +827,32 @@
       <c r="F7" s="1">
         <v>54274065976.905891</v>
       </c>
-      <c r="G7" s="2">
-        <f>D7/D$2</f>
+      <c r="G7" s="5">
+        <v>7575.8889960000006</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="0"/>
         <v>1.1668638293896183</v>
       </c>
-      <c r="H7" s="2">
-        <f>E7/E$2</f>
+      <c r="I7" s="2">
+        <f t="shared" si="1"/>
         <v>1.202672302045076</v>
       </c>
-      <c r="I7" s="2">
-        <f>F7/F$2</f>
+      <c r="J7" s="2">
+        <f t="shared" si="2"/>
         <v>1.009041964095871</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K7" s="2">
+        <f t="shared" si="2"/>
+        <v>1.138618658679319</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1966</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -784,25 +867,32 @@
       <c r="F8" s="1">
         <v>53803204978.332558</v>
       </c>
-      <c r="G8" s="2">
-        <f>D8/D$2</f>
+      <c r="G8" s="5">
+        <v>7566.0081480000008</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="0"/>
         <v>1.1895949730306619</v>
       </c>
-      <c r="H8" s="2">
-        <f>E8/E$2</f>
+      <c r="I8" s="2">
+        <f t="shared" si="1"/>
         <v>1.2491215483682467</v>
       </c>
-      <c r="I8" s="2">
-        <f>F8/F$2</f>
+      <c r="J8" s="2">
+        <f t="shared" si="2"/>
         <v>1.0002879026806317</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K8" s="2">
+        <f t="shared" si="2"/>
+        <v>1.1371336160787324</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1967</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -817,25 +907,32 @@
       <c r="F9" s="1">
         <v>52573053579.082481</v>
       </c>
-      <c r="G9" s="2">
-        <f>D9/D$2</f>
+      <c r="G9" s="5">
+        <v>7696.0501560000002</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="0"/>
         <v>1.2161145584744355</v>
       </c>
-      <c r="H9" s="2">
-        <f>E9/E$2</f>
+      <c r="I9" s="2">
+        <f t="shared" si="1"/>
         <v>1.3004149987917757</v>
       </c>
-      <c r="I9" s="2">
-        <f>F9/F$2</f>
+      <c r="J9" s="2">
+        <f t="shared" si="2"/>
         <v>0.97741741450746344</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K9" s="2">
+        <f t="shared" si="2"/>
+        <v>1.1566782869152645</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>1968</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -850,25 +947,32 @@
       <c r="F10" s="1">
         <v>52029784135.684921</v>
       </c>
-      <c r="G10" s="2">
-        <f>D10/D$2</f>
+      <c r="G10" s="5">
+        <v>7873.6542120000004</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="0"/>
         <v>1.3032504941060137</v>
       </c>
-      <c r="H10" s="2">
-        <f>E10/E$2</f>
+      <c r="I10" s="2">
+        <f t="shared" si="1"/>
         <v>1.3573592368624992</v>
       </c>
-      <c r="I10" s="2">
-        <f>F10/F$2</f>
+      <c r="J10" s="2">
+        <f t="shared" si="2"/>
         <v>0.96731716393046785</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K10" s="2">
+        <f t="shared" si="2"/>
+        <v>1.183371298405467</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>1969</v>
       </c>
       <c r="B11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -883,25 +987,32 @@
       <c r="F11" s="1">
         <v>51975173106.079163</v>
       </c>
-      <c r="G11" s="2">
-        <f>D11/D$2</f>
+      <c r="G11" s="5">
+        <v>8256.9138839999996</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="0"/>
         <v>1.2918849715679577</v>
       </c>
-      <c r="H11" s="2">
-        <f>E11/E$2</f>
+      <c r="I11" s="2">
+        <f t="shared" si="1"/>
         <v>1.4111211671397001</v>
       </c>
-      <c r="I11" s="2">
-        <f>F11/F$2</f>
+      <c r="J11" s="2">
+        <f t="shared" si="2"/>
         <v>0.96630185727188544</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K11" s="2">
+        <f t="shared" si="2"/>
+        <v>1.2409733321587233</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>1970</v>
       </c>
       <c r="B12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -916,25 +1027,32 @@
       <c r="F12" s="1">
         <v>50759575507.354767</v>
       </c>
-      <c r="G12" s="2">
-        <f>D12/D$2</f>
+      <c r="G12" s="5">
+        <v>8587.7966880000004</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="0"/>
         <v>1.3184045570117311</v>
       </c>
-      <c r="H12" s="2">
-        <f>E12/E$2</f>
+      <c r="I12" s="2">
+        <f t="shared" si="1"/>
         <v>1.4591718735381862</v>
       </c>
-      <c r="I12" s="2">
-        <f>F12/F$2</f>
+      <c r="J12" s="2">
+        <f t="shared" si="2"/>
         <v>0.94370194760068049</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K12" s="2">
+        <f t="shared" si="2"/>
+        <v>1.290703381618193</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>1971</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -949,25 +1067,32 @@
       <c r="F13" s="1">
         <v>49239298129.406029</v>
       </c>
-      <c r="G13" s="2">
-        <f>D13/D$2</f>
+      <c r="G13" s="5">
+        <v>8736.8467680000012</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="0"/>
         <v>1.3448324718294427</v>
       </c>
-      <c r="H13" s="2">
-        <f>E13/E$2</f>
+      <c r="I13" s="2">
+        <f t="shared" si="1"/>
         <v>1.5093881782128387</v>
       </c>
-      <c r="I13" s="2">
-        <f>F13/F$2</f>
+      <c r="J13" s="2">
+        <f t="shared" si="2"/>
         <v>0.91543755200392063</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K13" s="2">
+        <f t="shared" si="2"/>
+        <v>1.3131048716948366</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>1972</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -982,25 +1107,32 @@
       <c r="F14" s="1">
         <v>48718779753.475166</v>
       </c>
-      <c r="G14" s="2">
-        <f>D14/D$2</f>
+      <c r="G14" s="5">
+        <v>8800.9885439999998</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="0"/>
         <v>1.3936010871980891</v>
       </c>
-      <c r="H14" s="2">
-        <f>E14/E$2</f>
+      <c r="I14" s="2">
+        <f t="shared" si="1"/>
         <v>1.5568015025007491</v>
       </c>
-      <c r="I14" s="2">
-        <f>F14/F$2</f>
+      <c r="J14" s="2">
+        <f t="shared" si="2"/>
         <v>0.90576028027305822</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K14" s="2">
+        <f t="shared" si="2"/>
+        <v>1.3227450634918636</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>1973</v>
       </c>
       <c r="B15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1015,25 +1147,32 @@
       <c r="F15" s="1">
         <v>50039559418.106064</v>
       </c>
-      <c r="G15" s="2">
-        <f>D15/D$2</f>
+      <c r="G15" s="5">
+        <v>9130.1966279999997</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="0"/>
         <v>1.4955224395733955</v>
       </c>
-      <c r="H15" s="2">
-        <f>E15/E$2</f>
+      <c r="I15" s="2">
+        <f t="shared" si="1"/>
         <v>1.6088023770250266</v>
       </c>
-      <c r="I15" s="2">
-        <f>F15/F$2</f>
+      <c r="J15" s="2">
+        <f t="shared" si="2"/>
         <v>0.93031569330410202</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K15" s="2">
+        <f t="shared" si="2"/>
+        <v>1.3722234108156406</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>1974</v>
       </c>
       <c r="B16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1048,25 +1187,32 @@
       <c r="F16" s="1">
         <v>49138073677.692482</v>
       </c>
-      <c r="G16" s="2">
-        <f>D16/D$2</f>
+      <c r="G16" s="5">
+        <v>8792.6986800000013</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="0"/>
         <v>1.4704021806343623</v>
       </c>
-      <c r="H16" s="2">
-        <f>E16/E$2</f>
+      <c r="I16" s="2">
+        <f t="shared" si="1"/>
         <v>1.6550111792019315</v>
       </c>
-      <c r="I16" s="2">
-        <f>F16/F$2</f>
+      <c r="J16" s="2">
+        <f t="shared" si="2"/>
         <v>0.91355562704154492</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K16" s="2">
+        <f t="shared" si="2"/>
+        <v>1.3214991379201855</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>1975</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -1081,25 +1227,32 @@
       <c r="F17" s="1">
         <v>47946126425.399841</v>
       </c>
-      <c r="G17" s="2">
-        <f>D17/D$2</f>
+      <c r="G17" s="5">
+        <v>8347.0556880000004</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="0"/>
         <v>1.4604494664471865</v>
       </c>
-      <c r="H17" s="2">
-        <f>E17/E$2</f>
+      <c r="I17" s="2">
+        <f t="shared" si="1"/>
         <v>1.6974069954937985</v>
       </c>
-      <c r="I17" s="2">
-        <f>F17/F$2</f>
+      <c r="J17" s="2">
+        <f t="shared" si="2"/>
         <v>0.89139541525524146</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K17" s="2">
+        <f t="shared" si="2"/>
+        <v>1.2545211996123788</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>1976</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -1114,25 +1267,32 @@
       <c r="F18" s="1">
         <v>47389663450.660645</v>
       </c>
-      <c r="G18" s="2">
-        <f>D18/D$2</f>
+      <c r="G18" s="5">
+        <v>8512.4761560000006</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="0"/>
         <v>1.5014100496135276</v>
       </c>
-      <c r="H18" s="2">
-        <f>E18/E$2</f>
+      <c r="I18" s="2">
+        <f t="shared" si="1"/>
         <v>1.7388336307616417</v>
       </c>
-      <c r="I18" s="2">
-        <f>F18/F$2</f>
+      <c r="J18" s="2">
+        <f t="shared" si="2"/>
         <v>0.88104987576283655</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K18" s="2">
+        <f t="shared" si="2"/>
+        <v>1.2793830780654174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>1977</v>
       </c>
       <c r="B19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -1147,25 +1307,32 @@
       <c r="F19" s="1">
         <v>47301996228.218002</v>
       </c>
-      <c r="G19" s="2">
-        <f>D19/D$2</f>
+      <c r="G19" s="5">
+        <v>8694.1832759999998</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="0"/>
         <v>1.5368936393202706</v>
       </c>
-      <c r="H19" s="2">
-        <f>E19/E$2</f>
+      <c r="I19" s="2">
+        <f t="shared" si="1"/>
         <v>1.7787755759577868</v>
       </c>
-      <c r="I19" s="2">
-        <f>F19/F$2</f>
+      <c r="J19" s="2">
+        <f t="shared" si="2"/>
         <v>0.87942000144389398</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K19" s="2">
+        <f t="shared" si="2"/>
+        <v>1.3066927597880666</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>1978</v>
       </c>
       <c r="B20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -1180,25 +1347,32 @@
       <c r="F20" s="1">
         <v>47333580977.096489</v>
       </c>
-      <c r="G20" s="2">
-        <f>D20/D$2</f>
+      <c r="G20" s="5">
+        <v>8647.709796000001</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="0"/>
         <v>1.5891998744551401</v>
       </c>
-      <c r="H20" s="2">
-        <f>E20/E$2</f>
+      <c r="I20" s="2">
+        <f t="shared" si="1"/>
         <v>1.8220759345227464</v>
       </c>
-      <c r="I20" s="2">
-        <f>F20/F$2</f>
+      <c r="J20" s="2">
+        <f t="shared" si="2"/>
         <v>0.88000721260027537</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K20" s="2">
+        <f t="shared" si="2"/>
+        <v>1.2997080255225968</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>1979</v>
       </c>
       <c r="B21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -1213,25 +1387,32 @@
       <c r="F21" s="1">
         <v>47150212291.393204</v>
       </c>
-      <c r="G21" s="2">
-        <f>D21/D$2</f>
+      <c r="G21" s="5">
+        <v>9087.700608000001</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="0"/>
         <v>1.6328515755159112</v>
       </c>
-      <c r="H21" s="2">
-        <f>E21/E$2</f>
+      <c r="I21" s="2">
+        <f t="shared" si="1"/>
         <v>1.8645433937645619</v>
       </c>
-      <c r="I21" s="2">
-        <f>F21/F$2</f>
+      <c r="J21" s="2">
+        <f t="shared" si="2"/>
         <v>0.87659809453540716</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K21" s="2">
+        <f t="shared" si="2"/>
+        <v>1.3658364691224407</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>1980</v>
       </c>
       <c r="B22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -1246,25 +1427,32 @@
       <c r="F22" s="1">
         <v>46406215867.309525</v>
       </c>
-      <c r="G22" s="2">
-        <f>D22/D$2</f>
+      <c r="G22" s="5">
+        <v>8307.9509760000001</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="0"/>
         <v>1.5972700695499069</v>
       </c>
-      <c r="H22" s="2">
-        <f>E22/E$2</f>
+      <c r="I22" s="2">
+        <f t="shared" si="1"/>
         <v>1.8981535430490579</v>
       </c>
-      <c r="I22" s="2">
-        <f>F22/F$2</f>
+      <c r="J22" s="2">
+        <f t="shared" si="2"/>
         <v>0.86276600734007636</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K22" s="2">
+        <f t="shared" si="2"/>
+        <v>1.2486439547439561</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>1981</v>
       </c>
       <c r="B23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -1279,25 +1467,32 @@
       <c r="F23" s="1">
         <v>44102842860.298164</v>
       </c>
-      <c r="G23" s="2">
-        <f>D23/D$2</f>
+      <c r="G23" s="5">
+        <v>8057.4128640000008</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="0"/>
         <v>1.5761308693585638</v>
       </c>
-      <c r="H23" s="2">
-        <f>E23/E$2</f>
+      <c r="I23" s="2">
+        <f t="shared" si="1"/>
         <v>1.919599599960176</v>
       </c>
-      <c r="I23" s="2">
-        <f>F23/F$2</f>
+      <c r="J23" s="2">
+        <f t="shared" si="2"/>
         <v>0.81994260759646542</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K23" s="2">
+        <f t="shared" si="2"/>
+        <v>1.2109893152443398</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>1982</v>
       </c>
       <c r="B24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -1312,25 +1507,32 @@
       <c r="F24" s="1">
         <v>43067422476.234428</v>
       </c>
-      <c r="G24" s="2">
-        <f>D24/D$2</f>
+      <c r="G24" s="5">
+        <v>8012.1535560000002</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="0"/>
         <v>1.6091203731034411</v>
       </c>
-      <c r="H24" s="2">
-        <f>E24/E$2</f>
+      <c r="I24" s="2">
+        <f t="shared" si="1"/>
         <v>1.945367447784947</v>
       </c>
-      <c r="I24" s="2">
-        <f>F24/F$2</f>
+      <c r="J24" s="2">
+        <f t="shared" si="2"/>
         <v>0.80069248142303406</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K24" s="2">
+        <f t="shared" si="2"/>
+        <v>1.2041870650272468</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>1983</v>
       </c>
       <c r="B25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -1345,25 +1547,32 @@
       <c r="F25" s="1">
         <v>42656844020.519249</v>
       </c>
-      <c r="G25" s="2">
-        <f>D25/D$2</f>
+      <c r="G25" s="5">
+        <v>7967.8153440000006</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="0"/>
         <v>1.6674404701796426</v>
       </c>
-      <c r="H25" s="2">
-        <f>E25/E$2</f>
+      <c r="I25" s="2">
+        <f t="shared" si="1"/>
         <v>1.9754782992403945</v>
       </c>
-      <c r="I25" s="2">
-        <f>F25/F$2</f>
+      <c r="J25" s="2">
+        <f t="shared" si="2"/>
         <v>0.79305916919714381</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K25" s="2">
+        <f t="shared" si="2"/>
+        <v>1.1975232509847846</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>1984</v>
       </c>
       <c r="B26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -1378,25 +1587,32 @@
       <c r="F26" s="1">
         <v>43279519693.565422</v>
       </c>
-      <c r="G26" s="2">
-        <f>D26/D$2</f>
+      <c r="G26" s="5">
+        <v>7953.0359400000007</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="0"/>
         <v>1.7119765533394677</v>
       </c>
-      <c r="H26" s="2">
-        <f>E26/E$2</f>
+      <c r="I26" s="2">
+        <f t="shared" si="1"/>
         <v>2.0152263281837461</v>
       </c>
-      <c r="I26" s="2">
-        <f>F26/F$2</f>
+      <c r="J26" s="2">
+        <f t="shared" si="2"/>
         <v>0.80463570898306247</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K26" s="2">
+        <f t="shared" si="2"/>
+        <v>1.1953019796372972</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>1985</v>
       </c>
       <c r="B27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -1411,25 +1627,32 @@
       <c r="F27" s="1">
         <v>43965516047.096268</v>
       </c>
-      <c r="G27" s="2">
-        <f>D27/D$2</f>
+      <c r="G27" s="5">
+        <v>8406.4663799999998</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="0"/>
         <v>1.7735971194131637</v>
       </c>
-      <c r="H27" s="2">
-        <f>E27/E$2</f>
+      <c r="I27" s="2">
+        <f t="shared" si="1"/>
         <v>2.057182480897298</v>
       </c>
-      <c r="I27" s="2">
-        <f>F27/F$2</f>
+      <c r="J27" s="2">
+        <f t="shared" si="2"/>
         <v>0.81738948181121041</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K27" s="2">
+        <f t="shared" si="2"/>
+        <v>1.2634503328760744</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>1986</v>
       </c>
       <c r="B28" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -1444,25 +1667,32 @@
       <c r="F28" s="1">
         <v>43907934925.17466</v>
       </c>
-      <c r="G28" s="2">
-        <f>D28/D$2</f>
+      <c r="G28" s="5">
+        <v>8539.1460720000014</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" si="0"/>
         <v>1.8447596855689787</v>
       </c>
-      <c r="H28" s="2">
-        <f>E28/E$2</f>
+      <c r="I28" s="2">
+        <f t="shared" si="1"/>
         <v>2.1000894035974569</v>
       </c>
-      <c r="I28" s="2">
-        <f>F28/F$2</f>
+      <c r="J28" s="2">
+        <f t="shared" si="2"/>
         <v>0.8163189563712453</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K28" s="2">
+        <f t="shared" si="2"/>
+        <v>1.2833914345763227</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>1987</v>
       </c>
       <c r="B29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -1477,25 +1707,32 @@
       <c r="F29" s="1">
         <v>44600920610.96196</v>
       </c>
-      <c r="G29" s="2">
-        <f>D29/D$2</f>
+      <c r="G29" s="5">
+        <v>8606.0092679999998</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="0"/>
         <v>1.9289191139124675</v>
       </c>
-      <c r="H29" s="2">
-        <f>E29/E$2</f>
+      <c r="I29" s="2">
+        <f t="shared" si="1"/>
         <v>2.1496795328799614</v>
       </c>
-      <c r="I29" s="2">
-        <f>F29/F$2</f>
+      <c r="J29" s="2">
+        <f t="shared" si="2"/>
         <v>0.82920267209976062</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K29" s="2">
+        <f t="shared" si="2"/>
+        <v>1.2934406423438503</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>1988</v>
       </c>
       <c r="B30" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -1510,25 +1747,32 @@
       <c r="F30" s="1">
         <v>46407800398.139923</v>
       </c>
-      <c r="G30" s="2">
-        <f>D30/D$2</f>
+      <c r="G30" s="5">
+        <v>8683.6325400000005</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="0"/>
         <v>2.0259842872003548</v>
       </c>
-      <c r="H30" s="2">
-        <f>E30/E$2</f>
+      <c r="I30" s="2">
+        <f t="shared" si="1"/>
         <v>2.2164171420766752</v>
       </c>
-      <c r="I30" s="2">
-        <f>F30/F$2</f>
+      <c r="J30" s="2">
+        <f t="shared" si="2"/>
         <v>0.86279546631044268</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K30" s="2">
+        <f t="shared" si="2"/>
+        <v>1.3051070363332034</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>1989</v>
       </c>
       <c r="B31" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -1543,25 +1787,32 @@
       <c r="F31" s="1">
         <v>47488156941.223114</v>
       </c>
-      <c r="G31" s="2">
-        <f>D31/D$2</f>
+      <c r="G31" s="5">
+        <v>8665.545564</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="0"/>
         <v>2.0722060393414883</v>
       </c>
-      <c r="H31" s="2">
-        <f>E31/E$2</f>
+      <c r="I31" s="2">
+        <f t="shared" si="1"/>
         <v>2.289797733741378</v>
       </c>
-      <c r="I31" s="2">
-        <f>F31/F$2</f>
+      <c r="J31" s="2">
+        <f t="shared" si="2"/>
         <v>0.88288102777584587</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K31" s="2">
+        <f t="shared" si="2"/>
+        <v>1.3023886532677229</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>1990</v>
       </c>
       <c r="B32" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -1576,25 +1827,32 @@
       <c r="F32" s="1">
         <v>47434351552.677116</v>
       </c>
-      <c r="G32" s="2">
-        <f>D32/D$2</f>
+      <c r="G32" s="5">
+        <v>8621.4585600000009</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="0"/>
         <v>2.0883540394863274</v>
       </c>
-      <c r="H32" s="2">
-        <f>E32/E$2</f>
+      <c r="I32" s="2">
+        <f t="shared" si="1"/>
         <v>2.3540608594852612</v>
       </c>
-      <c r="I32" s="2">
-        <f>F32/F$2</f>
+      <c r="J32" s="2">
+        <f t="shared" si="2"/>
         <v>0.88188069927713897</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K32" s="2">
+        <f t="shared" si="2"/>
+        <v>1.2957625945456148</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>1991</v>
       </c>
       <c r="B33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -1609,25 +1867,32 @@
       <c r="F33" s="1">
         <v>45627257750.701874</v>
       </c>
-      <c r="G33" s="2">
-        <f>D33/D$2</f>
+      <c r="G33" s="5">
+        <v>8916.2092800000009</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" si="0"/>
         <v>2.0592749840512043</v>
       </c>
-      <c r="H33" s="2">
-        <f>E33/E$2</f>
+      <c r="I33" s="2">
+        <f t="shared" si="1"/>
         <v>2.4016087644542905</v>
       </c>
-      <c r="I33" s="2">
-        <f>F33/F$2</f>
+      <c r="J33" s="2">
+        <f t="shared" si="2"/>
         <v>0.84828392618800907</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K33" s="2">
+        <f t="shared" si="2"/>
+        <v>1.3400621704275162</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>1992</v>
       </c>
       <c r="B34" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -1642,25 +1907,32 @@
       <c r="F34" s="1">
         <v>44026099020.252312</v>
       </c>
-      <c r="G34" s="2">
-        <f>D34/D$2</f>
+      <c r="G34" s="5">
+        <v>8884.8920159999998</v>
+      </c>
+      <c r="H34" s="2">
+        <f t="shared" ref="H34:H52" si="4">D34/D$2</f>
         <v>2.0622945082184887</v>
       </c>
-      <c r="H34" s="2">
-        <f>E34/E$2</f>
+      <c r="I34" s="2">
+        <f t="shared" ref="I34:I52" si="5">E34/E$2</f>
         <v>2.4530916284312445</v>
       </c>
-      <c r="I34" s="2">
-        <f>F34/F$2</f>
+      <c r="J34" s="2">
+        <f t="shared" ref="J34:K52" si="6">F34/F$2</f>
         <v>0.81851581648180893</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K34" s="2">
+        <f t="shared" si="6"/>
+        <v>1.335355340490064</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>1993</v>
       </c>
       <c r="B35" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -1675,25 +1947,32 @@
       <c r="F35" s="1">
         <v>43572236175.19384</v>
       </c>
-      <c r="G35" s="2">
-        <f>D35/D$2</f>
+      <c r="G35" s="5">
+        <v>8970.7214160000003</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="4"/>
         <v>2.1081239500103601</v>
       </c>
-      <c r="H35" s="2">
-        <f>E35/E$2</f>
+      <c r="I35" s="2">
+        <f t="shared" si="5"/>
         <v>2.4999737342536852</v>
       </c>
-      <c r="I35" s="2">
-        <f>F35/F$2</f>
+      <c r="J35" s="2">
+        <f t="shared" si="6"/>
         <v>0.81007777801233427</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K35" s="2">
+        <f t="shared" si="6"/>
+        <v>1.348255074944311</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>1994</v>
       </c>
       <c r="B36" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -1708,25 +1987,32 @@
       <c r="F36" s="1">
         <v>44276189793.85379</v>
       </c>
-      <c r="G36" s="2">
-        <f>D36/D$2</f>
+      <c r="G36" s="5">
+        <v>9034.611984000001</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="4"/>
         <v>2.1983553301322138</v>
       </c>
-      <c r="H36" s="2">
-        <f>E36/E$2</f>
+      <c r="I36" s="2">
+        <f t="shared" si="5"/>
         <v>2.5523589391840407</v>
       </c>
-      <c r="I36" s="2">
-        <f>F36/F$2</f>
+      <c r="J36" s="2">
+        <f t="shared" si="6"/>
         <v>0.82316540520995896</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K36" s="2">
+        <f t="shared" si="6"/>
+        <v>1.3578575114209845</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>1995</v>
       </c>
       <c r="B37" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -1741,25 +2027,32 @@
       <c r="F37" s="1">
         <v>44856445163.726784</v>
       </c>
-      <c r="G37" s="2">
-        <f>D37/D$2</f>
+      <c r="G37" s="5">
+        <v>9054.5411519999998</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" si="4"/>
         <v>2.2652455100451023</v>
       </c>
-      <c r="H37" s="2">
-        <f>E37/E$2</f>
+      <c r="I37" s="2">
+        <f t="shared" si="5"/>
         <v>2.6097783621280959</v>
       </c>
-      <c r="I37" s="2">
-        <f>F37/F$2</f>
+      <c r="J37" s="2">
+        <f t="shared" si="6"/>
         <v>0.83395328350053988</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K37" s="2">
+        <f t="shared" si="6"/>
+        <v>1.3608527668357264</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>1996</v>
       </c>
       <c r="B38" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -1774,25 +2067,32 @@
       <c r="F38" s="1">
         <v>45252859756.469788</v>
       </c>
-      <c r="G38" s="2">
-        <f>D38/D$2</f>
+      <c r="G38" s="5">
+        <v>9444.3741000000009</v>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" si="4"/>
         <v>2.3304677382173318</v>
       </c>
-      <c r="H38" s="2">
-        <f>E38/E$2</f>
+      <c r="I38" s="2">
+        <f t="shared" si="5"/>
         <v>2.6728381664808052</v>
       </c>
-      <c r="I38" s="2">
-        <f>F38/F$2</f>
+      <c r="J38" s="2">
+        <f t="shared" si="6"/>
         <v>0.84132326678920433</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K38" s="2">
+        <f t="shared" si="6"/>
+        <v>1.4194427314715767</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>1997</v>
       </c>
       <c r="B39" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>37</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -1807,25 +2107,32 @@
       <c r="F39" s="1">
         <v>46047651512.146057</v>
       </c>
-      <c r="G39" s="2">
-        <f>D39/D$2</f>
+      <c r="G39" s="5">
+        <v>9179.684604</v>
+      </c>
+      <c r="H39" s="2">
+        <f t="shared" si="4"/>
         <v>2.407540269945573</v>
       </c>
-      <c r="H39" s="2">
-        <f>E39/E$2</f>
+      <c r="I39" s="2">
+        <f t="shared" si="5"/>
         <v>2.745852538596889</v>
       </c>
-      <c r="I39" s="2">
-        <f>F39/F$2</f>
+      <c r="J39" s="2">
+        <f t="shared" si="6"/>
         <v>0.85609972069512763</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K39" s="2">
+        <f t="shared" si="6"/>
+        <v>1.3796612089253577</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>1998</v>
       </c>
       <c r="B40" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -1840,25 +2147,32 @@
       <c r="F40" s="1">
         <v>46344767169.9524</v>
       </c>
-      <c r="G40" s="2">
-        <f>D40/D$2</f>
+      <c r="G40" s="5">
+        <v>9273.050244</v>
+      </c>
+      <c r="H40" s="2">
+        <f t="shared" si="4"/>
         <v>2.492157186046994</v>
       </c>
-      <c r="H40" s="2">
-        <f>E40/E$2</f>
+      <c r="I40" s="2">
+        <f t="shared" si="5"/>
         <v>2.8403734038556117</v>
       </c>
-      <c r="I40" s="2">
-        <f>F40/F$2</f>
+      <c r="J40" s="2">
+        <f t="shared" si="6"/>
         <v>0.86162357746760743</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K40" s="2">
+        <f t="shared" si="6"/>
+        <v>1.3936936029902214</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>1999</v>
       </c>
       <c r="B41" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -1873,25 +2187,32 @@
       <c r="F41" s="1">
         <v>46629025995.254555</v>
       </c>
-      <c r="G41" s="2">
-        <f>D41/D$2</f>
+      <c r="G41" s="5">
+        <v>9296.3707200000008</v>
+      </c>
+      <c r="H41" s="2">
+        <f t="shared" si="4"/>
         <v>2.5710770552206599</v>
       </c>
-      <c r="H41" s="2">
-        <f>E41/E$2</f>
+      <c r="I41" s="2">
+        <f t="shared" si="5"/>
         <v>2.9347027543012034</v>
       </c>
-      <c r="I41" s="2">
-        <f>F41/F$2</f>
+      <c r="J41" s="2">
+        <f t="shared" si="6"/>
         <v>0.86690840509626754</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K41" s="2">
+        <f t="shared" si="6"/>
+        <v>1.3971985552297412</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>2000</v>
       </c>
       <c r="B42" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="C42" s="1" t="s">
@@ -1906,25 +2227,32 @@
       <c r="F42" s="1">
         <v>46849046142.578064</v>
       </c>
-      <c r="G42" s="2">
-        <f>D42/D$2</f>
+      <c r="G42" s="5">
+        <v>9333.8844480000007</v>
+      </c>
+      <c r="H42" s="2">
+        <f t="shared" si="4"/>
         <v>2.6799740829872198</v>
       </c>
-      <c r="H42" s="2">
-        <f>E42/E$2</f>
+      <c r="I42" s="2">
+        <f t="shared" si="5"/>
         <v>3.0242022092244301</v>
       </c>
-      <c r="I42" s="2">
-        <f>F42/F$2</f>
+      <c r="J42" s="2">
+        <f t="shared" si="6"/>
         <v>0.87099893263644557</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K42" s="2">
+        <f t="shared" si="6"/>
+        <v>1.402836683069256</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>2001</v>
       </c>
       <c r="B43" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -1939,25 +2267,32 @@
       <c r="F43" s="1">
         <v>47310219736.099281</v>
       </c>
-      <c r="G43" s="2">
-        <f>D43/D$2</f>
+      <c r="G43" s="5">
+        <v>9368.8023599999997</v>
+      </c>
+      <c r="H43" s="2">
+        <f t="shared" si="4"/>
         <v>2.7573013736697853</v>
       </c>
-      <c r="H43" s="2">
-        <f>E43/E$2</f>
+      <c r="I43" s="2">
+        <f t="shared" si="5"/>
         <v>3.1082666058301953</v>
       </c>
-      <c r="I43" s="2">
-        <f>F43/F$2</f>
+      <c r="J43" s="2">
+        <f t="shared" si="6"/>
         <v>0.8795728896492444</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K43" s="2">
+        <f t="shared" si="6"/>
+        <v>1.4080846725984468</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>2002</v>
       </c>
       <c r="B44" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -1972,25 +2307,32 @@
       <c r="F44" s="1">
         <v>47157582601.165764</v>
       </c>
-      <c r="G44" s="2">
-        <f>D44/D$2</f>
+      <c r="G44" s="5">
+        <v>9146.1483360000002</v>
+      </c>
+      <c r="H44" s="2">
+        <f t="shared" si="4"/>
         <v>2.824384269012767</v>
       </c>
-      <c r="H44" s="2">
-        <f>E44/E$2</f>
+      <c r="I44" s="2">
+        <f t="shared" si="5"/>
         <v>3.1970836516491636</v>
       </c>
-      <c r="I44" s="2">
-        <f>F44/F$2</f>
+      <c r="J44" s="2">
+        <f t="shared" si="6"/>
         <v>0.87673512041904123</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K44" s="2">
+        <f t="shared" si="6"/>
+        <v>1.3746208736581129</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>2003</v>
       </c>
       <c r="B45" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="C45" s="1" t="s">
@@ -2005,25 +2347,32 @@
       <c r="F45" s="1">
         <v>47107782347.03067</v>
       </c>
-      <c r="G45" s="2">
-        <f>D45/D$2</f>
+      <c r="G45" s="5">
+        <v>9305.1211320000002</v>
+      </c>
+      <c r="H45" s="2">
+        <f t="shared" si="4"/>
         <v>2.9321315982609262</v>
       </c>
-      <c r="H45" s="2">
-        <f>E45/E$2</f>
+      <c r="I45" s="2">
+        <f t="shared" si="5"/>
         <v>3.2844198096759007</v>
       </c>
-      <c r="I45" s="2">
-        <f>F45/F$2</f>
+      <c r="J45" s="2">
+        <f t="shared" si="6"/>
         <v>0.87580925379489094</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K45" s="2">
+        <f t="shared" si="6"/>
+        <v>1.398513698888735</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>2004</v>
       </c>
       <c r="B46" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>44</v>
       </c>
       <c r="C46" s="1" t="s">
@@ -2038,25 +2387,32 @@
       <c r="F46" s="1">
         <v>47455324247.81794</v>
       </c>
-      <c r="G46" s="2">
-        <f>D46/D$2</f>
+      <c r="G46" s="5">
+        <v>9290.8441440000006</v>
+      </c>
+      <c r="H46" s="2">
+        <f t="shared" si="4"/>
         <v>3.0174016504866805</v>
       </c>
-      <c r="H46" s="2">
-        <f>E46/E$2</f>
+      <c r="I46" s="2">
+        <f t="shared" si="5"/>
         <v>3.3793058938833829</v>
       </c>
-      <c r="I46" s="2">
-        <f>F46/F$2</f>
+      <c r="J46" s="2">
+        <f t="shared" si="6"/>
         <v>0.8822706153285047</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K46" s="2">
+        <f t="shared" si="6"/>
+        <v>1.3963679381819556</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>2005</v>
       </c>
       <c r="B47" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="C47" s="1" t="s">
@@ -2071,25 +2427,32 @@
       <c r="F47" s="1">
         <v>48016605272.083313</v>
       </c>
-      <c r="G47" s="2">
-        <f>D47/D$2</f>
+      <c r="G47" s="5">
+        <v>9309.9359519999998</v>
+      </c>
+      <c r="H47" s="2">
+        <f t="shared" si="4"/>
         <v>3.1011126757328484</v>
       </c>
-      <c r="H47" s="2">
-        <f>E47/E$2</f>
+      <c r="I47" s="2">
+        <f t="shared" si="5"/>
         <v>3.4727583186120077</v>
       </c>
-      <c r="I47" s="2">
-        <f>F47/F$2</f>
+      <c r="J47" s="2">
+        <f t="shared" si="6"/>
         <v>0.89270573009170429</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K47" s="2">
+        <f t="shared" si="6"/>
+        <v>1.3992373425288513</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>2006</v>
       </c>
       <c r="B48" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>46</v>
       </c>
       <c r="C48" s="1" t="s">
@@ -2104,25 +2467,32 @@
       <c r="F48" s="1">
         <v>48274589085.90316</v>
       </c>
-      <c r="G48" s="2">
-        <f>D48/D$2</f>
+      <c r="G48" s="5">
+        <v>9168.4639800000004</v>
+      </c>
+      <c r="H48" s="2">
+        <f t="shared" si="4"/>
         <v>3.1817548559122559</v>
       </c>
-      <c r="H48" s="2">
-        <f>E48/E$2</f>
+      <c r="I48" s="2">
+        <f t="shared" si="5"/>
         <v>3.5745641512086497</v>
       </c>
-      <c r="I48" s="2">
-        <f>F48/F$2</f>
+      <c r="J48" s="2">
+        <f t="shared" si="6"/>
         <v>0.89750206310114733</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K48" s="2">
+        <f t="shared" si="6"/>
+        <v>1.3779748046162172</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>2007</v>
       </c>
       <c r="B49" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>47</v>
       </c>
       <c r="C49" s="1" t="s">
@@ -2137,25 +2507,32 @@
       <c r="F49" s="1">
         <v>48626446207.389915</v>
       </c>
-      <c r="G49" s="2">
-        <f>D49/D$2</f>
+      <c r="G49" s="5">
+        <v>8803.1238119999998</v>
+      </c>
+      <c r="H49" s="2">
+        <f t="shared" si="4"/>
         <v>3.2973375818608521</v>
       </c>
-      <c r="H49" s="2">
-        <f>E49/E$2</f>
+      <c r="I49" s="2">
+        <f t="shared" si="5"/>
         <v>3.6926881665558504</v>
       </c>
-      <c r="I49" s="2">
-        <f>F49/F$2</f>
+      <c r="J49" s="2">
+        <f t="shared" si="6"/>
         <v>0.90404365151092636</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K49" s="2">
+        <f t="shared" si="6"/>
+        <v>1.3230659837148717</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>2008</v>
       </c>
       <c r="B50" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>48</v>
       </c>
       <c r="C50" s="1" t="s">
@@ -2170,25 +2547,32 @@
       <c r="F50" s="1">
         <v>48354345642.757378</v>
       </c>
-      <c r="G50" s="2">
-        <f>D50/D$2</f>
+      <c r="G50" s="5">
+        <v>8714.531124000001</v>
+      </c>
+      <c r="H50" s="2">
+        <f t="shared" si="4"/>
         <v>3.2654233825766794</v>
       </c>
-      <c r="H50" s="2">
-        <f>E50/E$2</f>
+      <c r="I50" s="2">
+        <f t="shared" si="5"/>
         <v>3.793392138587083</v>
       </c>
-      <c r="I50" s="2">
-        <f>F50/F$2</f>
+      <c r="J50" s="2">
+        <f t="shared" si="6"/>
         <v>0.89898486545488931</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K50" s="2">
+        <f t="shared" si="6"/>
+        <v>1.3097509407367323</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>2009</v>
       </c>
       <c r="B51" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>49</v>
       </c>
       <c r="C51" s="1" t="s">
@@ -2203,25 +2587,32 @@
       <c r="F51" s="1">
         <v>47442570731.124863</v>
       </c>
-      <c r="G51" s="2">
-        <f>D51/D$2</f>
+      <c r="G51" s="5">
+        <v>8238.0314159999998</v>
+      </c>
+      <c r="H51" s="2">
+        <f t="shared" si="4"/>
         <v>3.1356416562738993</v>
       </c>
-      <c r="H51" s="2">
-        <f>E51/E$2</f>
+      <c r="I51" s="2">
+        <f t="shared" si="5"/>
         <v>3.8462978555644107</v>
       </c>
-      <c r="I51" s="2">
-        <f>F51/F$2</f>
+      <c r="J51" s="2">
+        <f t="shared" si="6"/>
         <v>0.88203350699137395</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K51" s="2">
+        <f t="shared" si="6"/>
+        <v>1.2381353905787891</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>2010</v>
       </c>
       <c r="B52" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="C52" s="1" t="s">
@@ -2236,50 +2627,24 @@
       <c r="F52" s="1">
         <v>47685549169.921898</v>
       </c>
-      <c r="G52" s="2">
-        <f>D52/D$2</f>
+      <c r="G52" s="5">
+        <v>8550.8691120000003</v>
+      </c>
+      <c r="H52" s="2">
+        <f t="shared" si="4"/>
         <v>3.1920618807459125</v>
       </c>
-      <c r="H52" s="2">
-        <f>E52/E$2</f>
+      <c r="I52" s="2">
+        <f t="shared" si="5"/>
         <v>3.9055441737321526</v>
       </c>
-      <c r="I52" s="2">
-        <f>F52/F$2</f>
+      <c r="J52" s="2">
+        <f t="shared" si="6"/>
         <v>0.88655086600444355</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="1">
-        <v>2011</v>
-      </c>
-      <c r="B53" s="1">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D53" s="3">
-        <v>2002324.8881300499</v>
-      </c>
-      <c r="E53" s="3">
-        <v>4947837.5</v>
-      </c>
-      <c r="F53" s="1">
-        <v>47931413864.135719</v>
-      </c>
-      <c r="G53" s="2">
-        <f>D53/D$2</f>
-        <v>3.2162681790797971</v>
-      </c>
-      <c r="H53" s="2">
-        <f>E53/E$2</f>
-        <v>3.96064440632159</v>
-      </c>
-      <c r="I53" s="2">
-        <f>F53/F$2</f>
-        <v>0.89112188513643387</v>
+      <c r="K52" s="2">
+        <f t="shared" si="6"/>
+        <v>1.2851533495261707</v>
       </c>
     </row>
   </sheetData>

</xml_diff>